<commit_message>
MSFT, MU, OXY, XOM
</commit_message>
<xml_diff>
--- a/MSFT.xlsx
+++ b/MSFT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97878402-54F6-4173-8F2E-4567C32B1B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A7B801-1061-4BF8-9923-9A77D73E0E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{505C5DB6-6863-4712-9628-F26C757D37C6}"/>
   </bookViews>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
-        <v>282.3</v>
+        <v>291.91000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="M5" s="2">
         <f>PRODUCT(M4,M3)</f>
-        <v>2105111.1</v>
+        <v>2176772.87</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="M8" s="2">
         <f>SUM(M5,-M6,M7)</f>
-        <v>2050126.1</v>
+        <v>2121787.87</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1132,10 +1132,10 @@
   <dimension ref="A1:DH59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="U15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Q12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH51" sqref="AH51"/>
+      <selection pane="bottomRight" activeCell="AH47" sqref="AH47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4313,251 +4313,251 @@
       </c>
       <c r="AN28" s="5">
         <f>AM28*(1+$AH$46)</f>
-        <v>89209.796115016972</v>
+        <v>87959.191496582149</v>
       </c>
       <c r="AO28" s="5">
         <f t="shared" ref="AO28:CW28" si="85">AN28*(1+$AH$46)</f>
-        <v>95454.481843068163</v>
+        <v>92796.947028894167</v>
       </c>
       <c r="AP28" s="5">
         <f t="shared" si="85"/>
-        <v>102136.29557208293</v>
+        <v>97900.779115483339</v>
       </c>
       <c r="AQ28" s="5">
         <f t="shared" si="85"/>
-        <v>109285.83626212875</v>
+        <v>103285.32196683492</v>
       </c>
       <c r="AR28" s="5">
         <f t="shared" si="85"/>
-        <v>116935.84480047777</v>
+        <v>108966.01467501084</v>
       </c>
       <c r="AS28" s="5">
         <f t="shared" si="85"/>
-        <v>125121.35393651122</v>
+        <v>114959.14548213643</v>
       </c>
       <c r="AT28" s="5">
         <f t="shared" si="85"/>
-        <v>133879.848712067</v>
+        <v>121281.89848365393</v>
       </c>
       <c r="AU28" s="5">
         <f t="shared" si="85"/>
-        <v>143251.43812191169</v>
+        <v>127952.40290025489</v>
       </c>
       <c r="AV28" s="5">
         <f t="shared" si="85"/>
-        <v>153279.03879044551</v>
+        <v>134989.78505976891</v>
       </c>
       <c r="AW28" s="5">
         <f t="shared" si="85"/>
-        <v>164008.57150577669</v>
+        <v>142414.22323805621</v>
       </c>
       <c r="AX28" s="5">
         <f t="shared" si="85"/>
-        <v>175489.17151118108</v>
+        <v>150247.00551614928</v>
       </c>
       <c r="AY28" s="5">
         <f t="shared" si="85"/>
-        <v>187773.41351696377</v>
+        <v>158510.59081953746</v>
       </c>
       <c r="AZ28" s="5">
         <f t="shared" si="85"/>
-        <v>200917.55246315125</v>
+        <v>167228.67331461201</v>
       </c>
       <c r="BA28" s="5">
         <f t="shared" si="85"/>
-        <v>214981.78113557186</v>
+        <v>176426.25034691565</v>
       </c>
       <c r="BB28" s="5">
         <f t="shared" si="85"/>
-        <v>230030.50581506192</v>
+        <v>186129.69411599601</v>
       </c>
       <c r="BC28" s="5">
         <f t="shared" si="85"/>
-        <v>246132.64122211628</v>
+        <v>196366.82729237579</v>
       </c>
       <c r="BD28" s="5">
         <f t="shared" si="85"/>
-        <v>263361.92610766442</v>
+        <v>207167.00279345646</v>
       </c>
       <c r="BE28" s="5">
         <f t="shared" si="85"/>
-        <v>281797.26093520096</v>
+        <v>218561.18794709654</v>
       </c>
       <c r="BF28" s="5">
         <f t="shared" si="85"/>
-        <v>301523.06920066505</v>
+        <v>230582.05328418684</v>
       </c>
       <c r="BG28" s="5">
         <f t="shared" si="85"/>
-        <v>322629.68404471164</v>
+        <v>243264.06621481711</v>
       </c>
       <c r="BH28" s="5">
         <f t="shared" si="85"/>
-        <v>345213.76192784146</v>
+        <v>256643.58985663202</v>
       </c>
       <c r="BI28" s="5">
         <f t="shared" si="85"/>
-        <v>369378.72526279039</v>
+        <v>270758.98729874677</v>
       </c>
       <c r="BJ28" s="5">
         <f t="shared" si="85"/>
-        <v>395235.23603118572</v>
+        <v>285650.73160017782</v>
       </c>
       <c r="BK28" s="5">
         <f t="shared" si="85"/>
-        <v>422901.70255336876</v>
+        <v>301361.52183818759</v>
       </c>
       <c r="BL28" s="5">
         <f t="shared" si="85"/>
-        <v>452504.82173210458</v>
+        <v>317936.40553928789</v>
       </c>
       <c r="BM28" s="5">
         <f t="shared" si="85"/>
-        <v>484180.15925335191</v>
+        <v>335422.90784394869</v>
       </c>
       <c r="BN28" s="5">
         <f t="shared" si="85"/>
-        <v>518072.7704010866</v>
+        <v>353871.16777536587</v>
       </c>
       <c r="BO28" s="5">
         <f t="shared" si="85"/>
-        <v>554337.86432916275</v>
+        <v>373334.08200301096</v>
       </c>
       <c r="BP28" s="5">
         <f t="shared" si="85"/>
-        <v>593141.51483220421</v>
+        <v>393867.45651317656</v>
       </c>
       <c r="BQ28" s="5">
         <f t="shared" si="85"/>
-        <v>634661.42087045859</v>
+        <v>415530.16662140127</v>
       </c>
       <c r="BR28" s="5">
         <f t="shared" si="85"/>
-        <v>679087.72033139074</v>
+        <v>438384.32578557829</v>
       </c>
       <c r="BS28" s="5">
         <f t="shared" si="85"/>
-        <v>726623.86075458815</v>
+        <v>462495.46370378509</v>
       </c>
       <c r="BT28" s="5">
         <f t="shared" si="85"/>
-        <v>777487.53100740933</v>
+        <v>487932.71420749323</v>
       </c>
       <c r="BU28" s="5">
         <f t="shared" si="85"/>
-        <v>831911.65817792807</v>
+        <v>514769.01348890533</v>
       </c>
       <c r="BV28" s="5">
         <f t="shared" si="85"/>
-        <v>890145.47425038309</v>
+        <v>543081.30923079513</v>
       </c>
       <c r="BW28" s="5">
         <f t="shared" si="85"/>
-        <v>952455.65744790994</v>
+        <v>572950.78123848885</v>
       </c>
       <c r="BX28" s="5">
         <f t="shared" si="85"/>
-        <v>1019127.5534692637</v>
+        <v>604463.07420660567</v>
       </c>
       <c r="BY28" s="5">
         <f t="shared" si="85"/>
-        <v>1090466.4822121123</v>
+        <v>637708.54328796896</v>
       </c>
       <c r="BZ28" s="5">
         <f t="shared" si="85"/>
-        <v>1166799.1359669601</v>
+        <v>672782.51316880726</v>
       </c>
       <c r="CA28" s="5">
         <f t="shared" si="85"/>
-        <v>1248475.0754846474</v>
+        <v>709785.55139309156</v>
       </c>
       <c r="CB28" s="5">
         <f t="shared" si="85"/>
-        <v>1335868.3307685729</v>
+        <v>748823.75671971159</v>
       </c>
       <c r="CC28" s="5">
         <f t="shared" si="85"/>
-        <v>1429379.1139223732</v>
+        <v>790009.06333929568</v>
       </c>
       <c r="CD28" s="5">
         <f t="shared" si="85"/>
-        <v>1529435.6518969394</v>
+        <v>833459.56182295689</v>
       </c>
       <c r="CE28" s="5">
         <f t="shared" si="85"/>
-        <v>1636496.1475297252</v>
+        <v>879299.83772321942</v>
       </c>
       <c r="CF28" s="5">
         <f t="shared" si="85"/>
-        <v>1751050.8778568062</v>
+        <v>927661.32879799639</v>
       </c>
       <c r="CG28" s="5">
         <f t="shared" si="85"/>
-        <v>1873624.4393067828</v>
+        <v>978682.70188188611</v>
       </c>
       <c r="CH28" s="5">
         <f t="shared" si="85"/>
-        <v>2004778.1500582576</v>
+        <v>1032510.2504853898</v>
       </c>
       <c r="CI28" s="5">
         <f t="shared" si="85"/>
-        <v>2145112.6205623359</v>
+        <v>1089298.3142620863</v>
       </c>
       <c r="CJ28" s="5">
         <f t="shared" si="85"/>
-        <v>2295270.5040016994</v>
+        <v>1149209.7215465009</v>
       </c>
       <c r="CK28" s="5">
         <f t="shared" si="85"/>
-        <v>2455939.4392818185</v>
+        <v>1212416.2562315585</v>
       </c>
       <c r="CL28" s="5">
         <f t="shared" si="85"/>
-        <v>2627855.2000315459</v>
+        <v>1279099.1503242941</v>
       </c>
       <c r="CM28" s="5">
         <f t="shared" si="85"/>
-        <v>2811805.0640337542</v>
+        <v>1349449.6035921301</v>
       </c>
       <c r="CN28" s="5">
         <f t="shared" si="85"/>
-        <v>3008631.4185161171</v>
+        <v>1423669.3317896973</v>
       </c>
       <c r="CO28" s="5">
         <f t="shared" si="85"/>
-        <v>3219235.6178122456</v>
+        <v>1501971.1450381305</v>
       </c>
       <c r="CP28" s="5">
         <f t="shared" si="85"/>
-        <v>3444582.1110591032</v>
+        <v>1584579.5580152276</v>
       </c>
       <c r="CQ28" s="5">
         <f t="shared" si="85"/>
-        <v>3685702.8588332408</v>
+        <v>1671731.4337060649</v>
       </c>
       <c r="CR28" s="5">
         <f t="shared" si="85"/>
-        <v>3943702.0589515679</v>
+        <v>1763676.6625598983</v>
       </c>
       <c r="CS28" s="5">
         <f t="shared" si="85"/>
-        <v>4219761.2030781778</v>
+        <v>1860678.8790006926</v>
       </c>
       <c r="CT28" s="5">
         <f t="shared" si="85"/>
-        <v>4515144.4872936504</v>
+        <v>1963016.2173457306</v>
       </c>
       <c r="CU28" s="5">
         <f t="shared" si="85"/>
-        <v>4831204.6014042059</v>
+        <v>2070982.1092997456</v>
       </c>
       <c r="CV28" s="5">
         <f t="shared" si="85"/>
-        <v>5169388.9235025002</v>
+        <v>2184886.1253112317</v>
       </c>
       <c r="CW28" s="5">
         <f t="shared" si="85"/>
-        <v>5531246.1481476752</v>
+        <v>2305054.8622033494</v>
       </c>
       <c r="CX28" s="5"/>
       <c r="CY28" s="5"/>
@@ -4854,27 +4854,27 @@
         <v>0.21848522087833899</v>
       </c>
       <c r="K33" s="7">
-        <f t="shared" ref="K33:K35" si="101">(K6/G6)-1</f>
+        <f t="shared" ref="K33:K34" si="101">(K6/G6)-1</f>
         <v>0.28768796867741742</v>
       </c>
       <c r="L33" s="7">
-        <f t="shared" ref="L33:L35" si="102">(L6/H6)-1</f>
+        <f t="shared" ref="L33:L34" si="102">(L6/H6)-1</f>
         <v>0.22053710534351167</v>
       </c>
       <c r="M33" s="7">
-        <f t="shared" ref="M33:M35" si="103">(M6/I6)-1</f>
+        <f t="shared" ref="M33:M34" si="103">(M6/I6)-1</f>
         <v>0.20823359273388919</v>
       </c>
       <c r="N33" s="7">
-        <f t="shared" ref="N33:N35" si="104">(N6/J6)-1</f>
+        <f t="shared" ref="N33:N34" si="104">(N6/J6)-1</f>
         <v>0.12550881000000036</v>
       </c>
       <c r="O33" s="7">
-        <f t="shared" ref="O33:O35" si="105">(O6/K6)-1</f>
+        <f t="shared" ref="O33:O34" si="105">(O6/K6)-1</f>
         <v>0.12550881000000014</v>
       </c>
       <c r="P33" s="7">
-        <f t="shared" ref="P33:P35" si="106">(P6/L6)-1</f>
+        <f t="shared" ref="P33:P34" si="106">(P6/L6)-1</f>
         <v>0.12550881000000014</v>
       </c>
       <c r="W33" s="7"/>
@@ -4900,7 +4900,7 @@
         <v>0.26843847710134261</v>
       </c>
       <c r="AD33" s="7">
-        <f t="shared" ref="AD33:AE35" si="108">(AD6/AC6)-1</f>
+        <f t="shared" ref="AD33:AE34" si="108">(AD6/AC6)-1</f>
         <v>0.45264506150462802</v>
       </c>
       <c r="AE33" s="7">
@@ -5028,7 +5028,7 @@
         <v>-3.1362007168458828E-2</v>
       </c>
       <c r="Z35" s="7">
-        <f t="shared" ref="Z35:AM35" si="111">Z28/Y28-1</f>
+        <f t="shared" ref="Z35:AE35" si="111">Z28/Y28-1</f>
         <v>0.24100491747407382</v>
       </c>
       <c r="AA35" s="7">
@@ -5118,27 +5118,27 @@
         <v>0.15333070555774531</v>
       </c>
       <c r="K37" s="7">
-        <f t="shared" ref="K36:K37" si="113">(K11/G11)-1</f>
+        <f t="shared" ref="K37" si="113">(K11/G11)-1</f>
         <v>0.13470632530120485</v>
       </c>
       <c r="L37" s="7">
-        <f t="shared" ref="L36:L37" si="114">(L11/H11)-1</f>
+        <f t="shared" ref="L37" si="114">(L11/H11)-1</f>
         <v>1.3117950391644984E-2</v>
       </c>
       <c r="M37" s="7">
-        <f t="shared" ref="M36:M37" si="115">(M11/I11)-1</f>
+        <f t="shared" ref="M37" si="115">(M11/I11)-1</f>
         <v>8.5677148387096835E-2</v>
       </c>
       <c r="N37" s="7">
-        <f t="shared" ref="N36:N37" si="116">(N11/J11)-1</f>
+        <f t="shared" ref="N37" si="116">(N11/J11)-1</f>
         <v>0.12550881000000014</v>
       </c>
       <c r="O37" s="7">
-        <f t="shared" ref="O36:O37" si="117">(O11/K11)-1</f>
+        <f t="shared" ref="O37" si="117">(O11/K11)-1</f>
         <v>0.12550880999999992</v>
       </c>
       <c r="P37" s="7">
-        <f t="shared" ref="P36:P37" si="118">(P11/L11)-1</f>
+        <f t="shared" ref="P37" si="118">(P11/L11)-1</f>
         <v>0.12550881000000014</v>
       </c>
       <c r="W37" s="7"/>
@@ -5679,7 +5679,7 @@
         <v>70</v>
       </c>
       <c r="AH46" s="27">
-        <v>7.0000000000000007E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AJ46" s="1" t="s">
         <v>72</v>
@@ -5721,7 +5721,7 @@
         <v>69</v>
       </c>
       <c r="AH47" s="29">
-        <v>7.4999999999999997E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="48" spans="2:39" x14ac:dyDescent="0.2">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="AH48" s="31">
         <f>NPV(AH47,AF28:CW28)</f>
-        <v>2963933.9243122642</v>
+        <v>3285079.1773080197</v>
       </c>
       <c r="AI48" s="15"/>
     </row>
@@ -5800,7 +5800,7 @@
       <c r="AG49" s="30"/>
       <c r="AH49" s="31">
         <f>AH48/Main!M4</f>
-        <v>397.47001801156824</v>
+        <v>440.53629841866967</v>
       </c>
       <c r="AJ49" s="2"/>
     </row>
@@ -5856,8 +5856,8 @@
         <v>71</v>
       </c>
       <c r="AH51" s="33">
-        <f>(AH49/282.3)-1</f>
-        <v>0.40797030822376268</v>
+        <f>(AH49/Main!M3)-1</f>
+        <v>0.50915110280110176</v>
       </c>
     </row>
     <row r="52" spans="2:36" x14ac:dyDescent="0.2">

</xml_diff>